<commit_message>
Change columns order and add type for filter
</commit_message>
<xml_diff>
--- a/subscription_report/subscriptions_by_creation_date/template.xlsx
+++ b/subscription_report/subscriptions_by_creation_date/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\ConnectCustomSubscriptionReport\subscription_report\subscriptions_by_creation_date\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{651DB3C8-3545-4960-BD72-0A8160EB0375}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF0BF306-A539-4F2B-9AC5-91F5765DC8EE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Data" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$AE$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$AB$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -464,16 +464,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AE1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="X7" sqref="X7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="4" width="21.1796875" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="21.1796875" customWidth="1"/>
+    <col min="3" max="4" width="25.81640625" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="20" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1" outlineLevel="1"/>
     <col min="7" max="7" width="45.81640625" customWidth="1" outlineLevel="1"/>
     <col min="8" max="9" width="15" customWidth="1" outlineLevel="1"/>
@@ -493,10 +493,10 @@
     <col min="23" max="23" width="45.81640625" customWidth="1"/>
     <col min="24" max="25" width="20" customWidth="1" outlineLevel="1"/>
     <col min="26" max="26" width="45.81640625" customWidth="1"/>
-    <col min="27" max="28" width="25.81640625" customWidth="1" outlineLevel="1"/>
-    <col min="29" max="29" width="20" customWidth="1"/>
-    <col min="30" max="30" width="14" customWidth="1"/>
-    <col min="31" max="31" width="18.453125" customWidth="1"/>
+    <col min="27" max="27" width="14" customWidth="1"/>
+    <col min="28" max="28" width="18.453125" customWidth="1"/>
+    <col min="29" max="30" width="21.1796875" customWidth="1" outlineLevel="1"/>
+    <col min="31" max="31" width="21.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.35">
@@ -507,13 +507,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -579,23 +579,23 @@
         <v>14</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AE1" xr:uid="{444A851A-3A6C-984B-A410-97137E4DF2E6}"/>
+  <autoFilter ref="A1:AB1" xr:uid="{444A851A-3A6C-984B-A410-97137E4DF2E6}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>